<commit_message>
refactor products service and related components
</commit_message>
<xml_diff>
--- a/app/data/products/laptops.xlsx
+++ b/app/data/products/laptops.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mat/Desktop/hejx/app/data/products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95628231-D365-CB42-946E-04D7F37B0C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C487F2-C915-B647-9B99-51BBE4DAD1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0E83B25D-4F86-1D47-8A1E-69E7BF78B9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52F3A99B-7CF5-D842-9A26-3855DCDBA2BC}" name="Table1" displayName="Table1" ref="D1:D5" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52F3A99B-7CF5-D842-9A26-3855DCDBA2BC}" name="Table1" displayName="Table1" ref="D1:D5" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="D1:D5" xr:uid="{52F3A99B-7CF5-D842-9A26-3855DCDBA2BC}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{EF11F7EF-8AB0-BC4E-8A4C-095A17A3CB10}" name="Manufacturer"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F0C4788-66E3-5647-ADF7-A2899B017F43}" name="Table2" displayName="Table2" ref="F1:F13" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F0C4788-66E3-5647-ADF7-A2899B017F43}" name="Table2" displayName="Table2" ref="F1:F13" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="F1:F13" xr:uid="{0F0C4788-66E3-5647-ADF7-A2899B017F43}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{556CADCB-6281-4D4B-8FF2-DD95FD8431D4}" name="Model"/>
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BA1A2B-F124-5048-8A13-CC48B51B2A35}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +833,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="b">
-        <f>VLOOKUP($B$1,$D$2:$E$5,2,FALSE)</f>
+        <f>IF(B2=F11,FALSE,TRUE)</f>
         <v>1</v>
       </c>
       <c r="F13" t="s">
@@ -842,6 +842,12 @@
       <c r="G13" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="b">
+        <f>VLOOKUP($B$1,$D$2:$E$5,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add product weight, quantity and prices processing
</commit_message>
<xml_diff>
--- a/app/data/products/laptops.xlsx
+++ b/app/data/products/laptops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mat/Desktop/hejx/app/data/products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C487F2-C915-B647-9B99-51BBE4DAD1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E14F13-E817-584B-9611-7811E70FD793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0E83B25D-4F86-1D47-8A1E-69E7BF78B9A0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{0E83B25D-4F86-1D47-8A1E-69E7BF78B9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BA1A2B-F124-5048-8A13-CC48B51B2A35}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -778,7 +778,8 @@
         <v>26</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <f>B4*1.053</f>
+        <v>1.0529999999999999</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -797,7 +798,7 @@
       </c>
       <c r="C11">
         <f>B4</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -833,7 +834,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="b">
-        <f>IF(B2=F11,FALSE,TRUE)</f>
+        <f>VLOOKUP($B$1,$D$2:$E$5,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F13" t="s">
@@ -842,12 +843,6 @@
       <c r="G13" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" t="b">
-        <f>VLOOKUP($B$1,$D$2:$E$5,2,FALSE)</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>